<commit_message>
Some changes made to the hypernym graphs
</commit_message>
<xml_diff>
--- a/xlsxFiles/interviewXlsxFiles/list_of_verbs.xlsx
+++ b/xlsxFiles/interviewXlsxFiles/list_of_verbs.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2470" uniqueCount="101">
   <si>
     <t xml:space="preserve">Verbs1</t>
   </si>
@@ -299,6 +299,15 @@
     <t xml:space="preserve">To practie </t>
   </si>
   <si>
+    <t xml:space="preserve">database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deficiency</t>
+  </si>
+  <si>
     <t xml:space="preserve">To  describe</t>
   </si>
   <si>
@@ -306,6 +315,9 @@
   </si>
   <si>
     <t xml:space="preserve">To anlayze </t>
+  </si>
+  <si>
+    <t xml:space="preserve">separate</t>
   </si>
   <si>
     <t xml:space="preserve">To rocognize </t>
@@ -320,7 +332,16 @@
     <t xml:space="preserve">To illustratute </t>
   </si>
   <si>
+    <t xml:space="preserve">advantages</t>
+  </si>
+  <si>
     <t xml:space="preserve">To analyse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impoundment</t>
   </si>
   <si>
     <t xml:space="preserve">The same individuals if used in 3 departments; have been reduced to one only. No repetiotion of any of the individual.</t>
@@ -15953,21 +15974,21 @@
   </sheetPr>
   <dimension ref="A1:AE406"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D287" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G302" activeCellId="0" sqref="G302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="24" min="11" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="24" min="11" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.57085020242915"/>
   </cols>
@@ -31408,9 +31429,7 @@
         <v>-</v>
       </c>
       <c r="K187" s="8"/>
-      <c r="L187" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="L187" s="9"/>
       <c r="M187" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!G188</f>
         <v>To evaluate</v>
@@ -32772,7 +32791,9 @@
         <f aca="false">IF(A204="-","-",MID([1]'verbs and nouns'!B205,2,LEN([1]'verbs and nouns'!B205)-2))</f>
         <v>plan</v>
       </c>
-      <c r="C204" s="8"/>
+      <c r="C204" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="D204" s="9" t="s">
         <v>51</v>
       </c>
@@ -33615,9 +33636,11 @@
         <f aca="false">IF(I214="-","-",MID([1]'verbs and nouns'!F215,2,LEN([1]'verbs and nouns'!F215)-2))</f>
         <v>-</v>
       </c>
-      <c r="K214" s="8"/>
+      <c r="K214" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="L214" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="M214" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!G215</f>
@@ -33696,9 +33719,11 @@
         <f aca="false">IF(I215="-","-",MID([1]'verbs and nouns'!F216,2,LEN([1]'verbs and nouns'!F216)-2))</f>
         <v>-</v>
       </c>
-      <c r="K215" s="8"/>
+      <c r="K215" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="L215" s="9" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="M215" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!G216</f>
@@ -37733,7 +37758,7 @@
       </c>
       <c r="C265" s="8"/>
       <c r="D265" s="9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E265" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!C266</f>
@@ -39848,7 +39873,7 @@
       </c>
       <c r="C290" s="8"/>
       <c r="D290" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E290" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!C291</f>
@@ -40295,7 +40320,7 @@
       </c>
       <c r="O295" s="8"/>
       <c r="P295" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q295" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!I296</f>
@@ -40932,9 +40957,11 @@
         <f aca="false">IF(E303="-","-",MID([1]'verbs and nouns'!D304,2,LEN([1]'verbs and nouns'!D304)-2))</f>
         <v>-</v>
       </c>
-      <c r="G303" s="8"/>
+      <c r="G303" s="8" t="s">
+        <v>90</v>
+      </c>
       <c r="H303" s="9" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="I303" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!E304</f>
@@ -43193,7 +43220,7 @@
         <v>fatal flaws</v>
       </c>
       <c r="H330" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I330" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!E331</f>
@@ -44144,7 +44171,7 @@
       </c>
       <c r="K341" s="8"/>
       <c r="L341" s="9" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="M341" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!G342</f>
@@ -44711,7 +44738,7 @@
         <v>justification</v>
       </c>
       <c r="H348" s="9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I348" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!E349</f>
@@ -44876,7 +44903,7 @@
       </c>
       <c r="G350" s="8"/>
       <c r="H350" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I350" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!E351</f>
@@ -45747,7 +45774,9 @@
         <f aca="false">IF(A360="-","-",MID([1]'verbs and nouns'!B361,2,LEN([1]'verbs and nouns'!B361)-2))</f>
         <v>cut off grade reserve</v>
       </c>
-      <c r="C360" s="8"/>
+      <c r="C360" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="D360" s="9" t="s">
         <v>29</v>
       </c>
@@ -46598,7 +46627,7 @@
         <v>economic</v>
       </c>
       <c r="P369" s="9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="Q369" s="10" t="str">
         <f aca="false">[1]'verbs and nouns'!I370</f>
@@ -47307,7 +47336,9 @@
         <f aca="false">IF(E378="-","-",MID([1]'verbs and nouns'!D379,2,LEN([1]'verbs and nouns'!D379)-2))</f>
         <v>impoundment and dams</v>
       </c>
-      <c r="G378" s="8"/>
+      <c r="G378" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="H378" s="9" t="s">
         <v>52</v>
       </c>
@@ -47457,7 +47488,9 @@
         <f aca="false">IF(A380="-","-",MID([1]'verbs and nouns'!B381,2,LEN([1]'verbs and nouns'!B381)-2))</f>
         <v>a power ful engine</v>
       </c>
-      <c r="C380" s="8"/>
+      <c r="C380" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="D380" s="9" t="s">
         <v>52</v>
       </c>
@@ -49670,12 +49703,12 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>